<commit_message>
md file gemaakt van de mapping van Astrid
</commit_message>
<xml_diff>
--- a/maps/FamilyMemberHistory-FamilyHistory.xlsx
+++ b/maps/FamilyMemberHistory-FamilyHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/jacob_engel_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{40490518-20AA-47AF-A604-EDBE625C23C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C40505DA-4AC5-4E5F-9B72-41C1F4DD829F}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{40490518-20AA-47AF-A604-EDBE625C23C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5949838-7DBC-2241-941F-B60215A55101}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="2292" windowWidth="23208" windowHeight="12120" xr2:uid="{02FC4626-A12F-4F2B-A4F9-C91521D9ECCA}"/>
+    <workbookView xWindow="500" yWindow="700" windowWidth="23200" windowHeight="12120" xr2:uid="{02FC4626-A12F-4F2B-A4F9-C91521D9ECCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>xtehr</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>EHDSFamilyMemberHistory.causeOfDeath</t>
+  </si>
+  <si>
+    <t>FamilyHistory.FamilyMember.Disorder.DisorderFamilyMember.Diagnosis</t>
   </si>
 </sst>
 </file>
@@ -163,9 +166,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -500,19 +506,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8631DB2A-343D-442B-A304-5E36E8950659}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,141 +526,153 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>